<commit_message>
Convert Changes.rst to keepachangelog style
</commit_message>
<xml_diff>
--- a/tests/fixtures/basic.xlsx
+++ b/tests/fixtures/basic.xlsx
@@ -1,15 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFA1386-3D44-4221-BB37-6433D7ABE23D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="420" windowWidth="21795" windowHeight="8985"/>
+    <workbookView xWindow="39225" yWindow="5625" windowWidth="18780" windowHeight="16950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -28,8 +40,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +79,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -113,7 +133,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -145,9 +165,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,6 +217,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -354,14 +410,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -372,7 +428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -385,7 +441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -398,7 +454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -413,5 +469,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>